<commit_message>
lots of misc, start react version
</commit_message>
<xml_diff>
--- a/research/Paper3/Census data for research paper.xlsx
+++ b/research/Paper3/Census data for research paper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isabelle Sanford\Documents\Coding\senate-analysis\research\Paper3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F46AD010-905D-4BA8-8323-318F68B623EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52E06C3-2FAE-462E-AB2B-E95070E07F9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9D0763FF-026C-435A-964F-CC13DF11886A}"/>
   </bookViews>
@@ -230,8 +230,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="174" formatCode="0.000"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -292,17 +292,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="174" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -624,8 +624,8 @@
   <dimension ref="A1:K57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B52" sqref="B46:B52"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -645,7 +645,7 @@
       <c r="B1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="7">
+      <c r="D1" s="6">
         <v>3307597</v>
       </c>
       <c r="F1" t="s">
@@ -659,16 +659,16 @@
       <c r="B2" s="3">
         <v>576851</v>
       </c>
-      <c r="D2" s="8">
-        <f xml:space="preserve"> B2 / $D$1</f>
+      <c r="D2" s="7">
+        <f t="shared" ref="D2:D33" si="0" xml:space="preserve"> B2 / $D$1</f>
         <v>0.17440183915997021</v>
       </c>
       <c r="E2">
-        <f>IF(D2 &lt; 1, 1, ROUND(D2,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F2" s="13">
-        <f>B2 / E2</f>
+        <f t="shared" ref="E2:E33" si="1">IF(D2 &lt; 1, 1, ROUND(D2,0))</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="12">
+        <f t="shared" ref="F2:F33" si="2">B2 / E2</f>
         <v>576851</v>
       </c>
     </row>
@@ -679,37 +679,37 @@
       <c r="B3" s="3">
         <v>643077</v>
       </c>
-      <c r="D3" s="8">
-        <f xml:space="preserve"> B3 / $D$1</f>
+      <c r="D3" s="7">
+        <f t="shared" si="0"/>
         <v>0.19442423003769807</v>
       </c>
       <c r="E3">
-        <f>IF(D3 &lt; 1, 1, ROUND(D3,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F3" s="13">
-        <f>B3 / E3</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F3" s="12">
+        <f t="shared" si="2"/>
         <v>643077</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>689545</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12">
-        <f xml:space="preserve"> B4 / $D$1</f>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11">
+        <f t="shared" si="0"/>
         <v>0.20847309995746158</v>
       </c>
-      <c r="E4" s="11">
-        <f>IF(D4 &lt; 1, 1, ROUND(D4,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F4" s="13">
-        <f>B4 / E4</f>
+      <c r="E4" s="10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F4" s="12">
+        <f t="shared" si="2"/>
         <v>689545</v>
       </c>
     </row>
@@ -720,16 +720,16 @@
       <c r="B5" s="3">
         <v>733391</v>
       </c>
-      <c r="D5" s="8">
-        <f xml:space="preserve"> B5 / $D$1</f>
+      <c r="D5" s="7">
+        <f t="shared" si="0"/>
         <v>0.2217292493613944</v>
       </c>
       <c r="E5">
-        <f>IF(D5 &lt; 1, 1, ROUND(D5,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F5" s="13">
-        <f>B5 / E5</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F5" s="12">
+        <f t="shared" si="2"/>
         <v>733391</v>
       </c>
     </row>
@@ -740,19 +740,19 @@
       <c r="B6" s="3">
         <v>779094</v>
       </c>
-      <c r="D6" s="8">
-        <f xml:space="preserve"> B6 / $D$1</f>
+      <c r="D6" s="7">
+        <f t="shared" si="0"/>
         <v>0.23554683354713407</v>
       </c>
       <c r="E6">
-        <f>IF(D6 &lt; 1, 1, ROUND(D6,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F6" s="13">
-        <f>B6 / E6</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F6" s="12">
+        <f t="shared" si="2"/>
         <v>779094</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="13">
         <f>F2*20</f>
         <v>11537020</v>
       </c>
@@ -764,16 +764,16 @@
       <c r="B7" s="3">
         <v>886667</v>
       </c>
-      <c r="D7" s="8">
-        <f xml:space="preserve"> B7 / $D$1</f>
+      <c r="D7" s="7">
+        <f t="shared" si="0"/>
         <v>0.26806984043098359</v>
       </c>
       <c r="E7">
-        <f>IF(D7 &lt; 1, 1, ROUND(D7,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F7" s="13">
-        <f>B7 / E7</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F7" s="12">
+        <f t="shared" si="2"/>
         <v>886667</v>
       </c>
     </row>
@@ -784,16 +784,16 @@
       <c r="B8" s="3">
         <v>989948</v>
       </c>
-      <c r="D8" s="8">
-        <f xml:space="preserve"> B8 / $D$1</f>
+      <c r="D8" s="7">
+        <f t="shared" si="0"/>
         <v>0.29929522852995694</v>
       </c>
       <c r="E8">
-        <f>IF(D8 &lt; 1, 1, ROUND(D8,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F8" s="13">
-        <f>B8 / E8</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F8" s="12">
+        <f t="shared" si="2"/>
         <v>989948</v>
       </c>
     </row>
@@ -804,16 +804,16 @@
       <c r="B9" s="3">
         <v>1084225</v>
       </c>
-      <c r="D9" s="8">
-        <f xml:space="preserve"> B9 / $D$1</f>
+      <c r="D9" s="7">
+        <f t="shared" si="0"/>
         <v>0.32779839865618454</v>
       </c>
       <c r="E9">
-        <f>IF(D9 &lt; 1, 1, ROUND(D9,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F9" s="13">
-        <f>B9 / E9</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F9" s="12">
+        <f t="shared" si="2"/>
         <v>1084225</v>
       </c>
     </row>
@@ -824,16 +824,16 @@
       <c r="B10" s="3">
         <v>1097379</v>
       </c>
-      <c r="D10" s="8">
-        <f xml:space="preserve"> B10 / $D$1</f>
+      <c r="D10" s="7">
+        <f t="shared" si="0"/>
         <v>0.33177530394422294</v>
       </c>
       <c r="E10">
-        <f>IF(D10 &lt; 1, 1, ROUND(D10,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F10" s="13">
-        <f>B10 / E10</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F10" s="12">
+        <f t="shared" si="2"/>
         <v>1097379</v>
       </c>
     </row>
@@ -844,16 +844,16 @@
       <c r="B11" s="3">
         <v>1362359</v>
       </c>
-      <c r="D11" s="8">
-        <f xml:space="preserve"> B11 / $D$1</f>
+      <c r="D11" s="7">
+        <f t="shared" si="0"/>
         <v>0.4118878448613903</v>
       </c>
       <c r="E11">
-        <f>IF(D11 &lt; 1, 1, ROUND(D11,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F11" s="13">
-        <f>B11 / E11</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F11" s="12">
+        <f t="shared" si="2"/>
         <v>1362359</v>
       </c>
     </row>
@@ -864,16 +864,16 @@
       <c r="B12" s="3">
         <v>1377529</v>
       </c>
-      <c r="D12" s="8">
-        <f xml:space="preserve"> B12 / $D$1</f>
+      <c r="D12" s="7">
+        <f t="shared" si="0"/>
         <v>0.4164742560837974</v>
       </c>
       <c r="E12">
-        <f>IF(D12 &lt; 1, 1, ROUND(D12,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F12" s="13">
-        <f>B12 / E12</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F12" s="12">
+        <f t="shared" si="2"/>
         <v>1377529</v>
       </c>
       <c r="J12">
@@ -888,16 +888,16 @@
       <c r="B13" s="3">
         <v>1455271</v>
       </c>
-      <c r="D13" s="8">
-        <f xml:space="preserve"> B13 / $D$1</f>
+      <c r="D13" s="7">
+        <f t="shared" si="0"/>
         <v>0.43997832867788911</v>
       </c>
       <c r="E13">
-        <f>IF(D13 &lt; 1, 1, ROUND(D13,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F13" s="13">
-        <f>B13 / E13</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F13" s="12">
+        <f t="shared" si="2"/>
         <v>1455271</v>
       </c>
     </row>
@@ -908,16 +908,16 @@
       <c r="B14" s="3">
         <v>1793716</v>
       </c>
-      <c r="D14" s="8">
-        <f xml:space="preserve"> B14 / $D$1</f>
+      <c r="D14" s="7">
+        <f t="shared" si="0"/>
         <v>0.54230185841866463</v>
       </c>
       <c r="E14">
-        <f>IF(D14 &lt; 1, 1, ROUND(D14,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F14" s="13">
-        <f>B14 / E14</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F14" s="12">
+        <f t="shared" si="2"/>
         <v>1793716</v>
       </c>
     </row>
@@ -928,16 +928,16 @@
       <c r="B15" s="3">
         <v>1839106</v>
       </c>
-      <c r="D15" s="8">
-        <f xml:space="preserve"> B15 / $D$1</f>
+      <c r="D15" s="7">
+        <f t="shared" si="0"/>
         <v>0.55602481197074494</v>
       </c>
       <c r="E15">
-        <f>IF(D15 &lt; 1, 1, ROUND(D15,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F15" s="13">
-        <f>B15 / E15</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F15" s="12">
+        <f t="shared" si="2"/>
         <v>1839106</v>
       </c>
     </row>
@@ -948,16 +948,16 @@
       <c r="B16" s="3">
         <v>1961504</v>
       </c>
-      <c r="D16" s="8">
-        <f xml:space="preserve"> B16 / $D$1</f>
+      <c r="D16" s="7">
+        <f t="shared" si="0"/>
         <v>0.59302992474597116</v>
       </c>
       <c r="E16">
-        <f>IF(D16 &lt; 1, 1, ROUND(D16,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F16" s="13">
-        <f>B16 / E16</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F16" s="12">
+        <f t="shared" si="2"/>
         <v>1961504</v>
       </c>
     </row>
@@ -968,16 +968,16 @@
       <c r="B17" s="3">
         <v>2117522</v>
       </c>
-      <c r="D17" s="8">
-        <f xml:space="preserve"> B17 / $D$1</f>
+      <c r="D17" s="7">
+        <f t="shared" si="0"/>
         <v>0.64019951644653206</v>
       </c>
       <c r="E17">
-        <f>IF(D17 &lt; 1, 1, ROUND(D17,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F17" s="13">
-        <f>B17 / E17</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F17" s="12">
+        <f t="shared" si="2"/>
         <v>2117522</v>
       </c>
       <c r="I17">
@@ -992,16 +992,16 @@
       <c r="B18" s="3">
         <v>2937880</v>
       </c>
-      <c r="D18" s="8">
-        <f xml:space="preserve"> B18 / $D$1</f>
+      <c r="D18" s="7">
+        <f t="shared" si="0"/>
         <v>0.88822187225348193</v>
       </c>
       <c r="E18">
-        <f>IF(D18 &lt; 1, 1, ROUND(D18,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F18" s="13">
-        <f>B18 / E18</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F18" s="12">
+        <f t="shared" si="2"/>
         <v>2937880</v>
       </c>
     </row>
@@ -1012,16 +1012,16 @@
       <c r="B19" s="3">
         <v>2961279</v>
       </c>
-      <c r="D19" s="8">
-        <f xml:space="preserve"> B19 / $D$1</f>
+      <c r="D19" s="7">
+        <f t="shared" si="0"/>
         <v>0.89529619237168256</v>
       </c>
       <c r="E19">
-        <f>IF(D19 &lt; 1, 1, ROUND(D19,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F19" s="13">
-        <f>B19 / E19</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F19" s="12">
+        <f t="shared" si="2"/>
         <v>2961279</v>
       </c>
     </row>
@@ -1032,16 +1032,16 @@
       <c r="B20" s="3">
         <v>3011524</v>
       </c>
-      <c r="D20" s="8">
-        <f xml:space="preserve"> B20 / $D$1</f>
+      <c r="D20" s="7">
+        <f t="shared" si="0"/>
         <v>0.91048697891550878</v>
       </c>
       <c r="E20">
-        <f>IF(D20 &lt; 1, 1, ROUND(D20,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F20" s="13">
-        <f>B20 / E20</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F20" s="12">
+        <f t="shared" si="2"/>
         <v>3011524</v>
       </c>
     </row>
@@ -1052,16 +1052,16 @@
       <c r="B21" s="3">
         <v>3104614</v>
       </c>
-      <c r="D21" s="8">
-        <f xml:space="preserve"> B21 / $D$1</f>
+      <c r="D21" s="7">
+        <f t="shared" si="0"/>
         <v>0.93863127823613335</v>
       </c>
       <c r="E21">
-        <f>IF(D21 &lt; 1, 1, ROUND(D21,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F21" s="13">
-        <f>B21 / E21</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F21" s="12">
+        <f t="shared" si="2"/>
         <v>3104614</v>
       </c>
     </row>
@@ -1072,16 +1072,16 @@
       <c r="B22" s="3">
         <v>3190369</v>
       </c>
-      <c r="D22" s="8">
-        <f xml:space="preserve"> B22 / $D$1</f>
+      <c r="D22" s="7">
+        <f t="shared" si="0"/>
         <v>0.96455795551876489</v>
       </c>
       <c r="E22">
-        <f>IF(D22 &lt; 1, 1, ROUND(D22,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F22" s="13">
-        <f>B22 / E22</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F22" s="12">
+        <f t="shared" si="2"/>
         <v>3190369</v>
       </c>
     </row>
@@ -1092,16 +1092,16 @@
       <c r="B23" s="3">
         <v>3271616</v>
       </c>
-      <c r="D23" s="8">
-        <f xml:space="preserve"> B23 / $D$1</f>
+      <c r="D23" s="7">
+        <f t="shared" si="0"/>
         <v>0.98912170980926639</v>
       </c>
       <c r="E23">
-        <f>IF(D23 &lt; 1, 1, ROUND(D23,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F23" s="13">
-        <f>B23 / E23</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F23" s="12">
+        <f t="shared" si="2"/>
         <v>3271616</v>
       </c>
     </row>
@@ -1112,16 +1112,16 @@
       <c r="B24" s="3">
         <v>3605944</v>
       </c>
-      <c r="D24" s="8">
-        <f xml:space="preserve"> B24 / $D$1</f>
+      <c r="D24" s="7">
+        <f t="shared" si="0"/>
         <v>1.090200529266413</v>
       </c>
       <c r="E24">
-        <f>IF(D24 &lt; 1, 1, ROUND(D24,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F24" s="13">
-        <f>B24 / E24</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F24" s="12">
+        <f t="shared" si="2"/>
         <v>3605944</v>
       </c>
     </row>
@@ -1132,16 +1132,16 @@
       <c r="B25" s="3">
         <v>3959353</v>
       </c>
-      <c r="D25" s="8">
-        <f xml:space="preserve"> B25 / $D$1</f>
+      <c r="D25" s="7">
+        <f t="shared" si="0"/>
         <v>1.1970481893652702</v>
       </c>
       <c r="E25">
-        <f>IF(D25 &lt; 1, 1, ROUND(D25,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F25" s="13">
-        <f>B25 / E25</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F25" s="12">
+        <f t="shared" si="2"/>
         <v>3959353</v>
       </c>
     </row>
@@ -1152,16 +1152,16 @@
       <c r="B26" s="3">
         <v>4237256</v>
       </c>
-      <c r="D26" s="8">
-        <f xml:space="preserve"> B26 / $D$1</f>
+      <c r="D26" s="7">
+        <f t="shared" si="0"/>
         <v>1.2810677963488297</v>
       </c>
       <c r="E26">
-        <f>IF(D26 &lt; 1, 1, ROUND(D26,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F26" s="13">
-        <f>B26 / E26</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F26" s="12">
+        <f t="shared" si="2"/>
         <v>4237256</v>
       </c>
     </row>
@@ -1172,16 +1172,16 @@
       <c r="B27" s="3">
         <v>4505836</v>
       </c>
-      <c r="D27" s="8">
-        <f xml:space="preserve"> B27 / $D$1</f>
+      <c r="D27" s="7">
+        <f t="shared" si="0"/>
         <v>1.3622687407202267</v>
       </c>
       <c r="E27">
-        <f>IF(D27 &lt; 1, 1, ROUND(D27,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F27" s="13">
-        <f>B27 / E27</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F27" s="12">
+        <f t="shared" si="2"/>
         <v>4505836</v>
       </c>
     </row>
@@ -1192,16 +1192,16 @@
       <c r="B28" s="3">
         <v>4657757</v>
       </c>
-      <c r="D28" s="8">
-        <f xml:space="preserve"> B28 / $D$1</f>
+      <c r="D28" s="7">
+        <f t="shared" si="0"/>
         <v>1.4081996688230156</v>
       </c>
       <c r="E28">
-        <f>IF(D28 &lt; 1, 1, ROUND(D28,0))</f>
-        <v>1</v>
-      </c>
-      <c r="F28" s="13">
-        <f>B28 / E28</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F28" s="12">
+        <f t="shared" si="2"/>
         <v>4657757</v>
       </c>
     </row>
@@ -1212,20 +1212,20 @@
       <c r="B29" s="3">
         <v>5024279</v>
       </c>
-      <c r="D29" s="8">
-        <f xml:space="preserve"> B29 / $D$1</f>
+      <c r="D29" s="7">
+        <f t="shared" si="0"/>
         <v>1.5190118385039049</v>
       </c>
       <c r="E29">
-        <f>IF(D29 &lt; 1, 1, ROUND(D29,0))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F29" s="13">
-        <f>B29 / E29</f>
+      <c r="F29" s="12">
+        <f t="shared" si="2"/>
         <v>2512139.5</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>41</v>
       </c>
@@ -1233,16 +1233,16 @@
         <v>5118425</v>
       </c>
       <c r="C30"/>
-      <c r="D30" s="8">
-        <f xml:space="preserve"> B30 / $D$1</f>
+      <c r="D30" s="7">
+        <f t="shared" si="0"/>
         <v>1.5474754028377702</v>
       </c>
       <c r="E30">
-        <f>IF(D30 &lt; 1, 1, ROUND(D30,0))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F30" s="13">
-        <f>B30 / E30</f>
+      <c r="F30" s="12">
+        <f t="shared" si="2"/>
         <v>2559212.5</v>
       </c>
     </row>
@@ -1253,16 +1253,16 @@
       <c r="B31" s="3">
         <v>5706494</v>
       </c>
-      <c r="D31" s="8">
-        <f xml:space="preserve"> B31 / $D$1</f>
+      <c r="D31" s="7">
+        <f t="shared" si="0"/>
         <v>1.7252688280948374</v>
       </c>
       <c r="E31">
-        <f>IF(D31 &lt; 1, 1, ROUND(D31,0))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F31" s="13">
-        <f>B31 / E31</f>
+      <c r="F31" s="12">
+        <f t="shared" si="2"/>
         <v>2853247</v>
       </c>
     </row>
@@ -1273,16 +1273,16 @@
       <c r="B32" s="3">
         <v>5773714</v>
       </c>
-      <c r="D32" s="8">
-        <f xml:space="preserve"> B32 / $D$1</f>
+      <c r="D32" s="7">
+        <f t="shared" si="0"/>
         <v>1.7455917392596498</v>
       </c>
       <c r="E32">
-        <f>IF(D32 &lt; 1, 1, ROUND(D32,0))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F32" s="13">
-        <f>B32 / E32</f>
+      <c r="F32" s="12">
+        <f t="shared" si="2"/>
         <v>2886857</v>
       </c>
     </row>
@@ -1293,16 +1293,16 @@
       <c r="B33" s="3">
         <v>5893718</v>
       </c>
-      <c r="D33" s="8">
-        <f xml:space="preserve"> B33 / $D$1</f>
+      <c r="D33" s="7">
+        <f t="shared" si="0"/>
         <v>1.7818730637378133</v>
       </c>
       <c r="E33">
-        <f>IF(D33 &lt; 1, 1, ROUND(D33,0))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F33" s="13">
-        <f>B33 / E33</f>
+      <c r="F33" s="12">
+        <f t="shared" si="2"/>
         <v>2946859</v>
       </c>
     </row>
@@ -1313,16 +1313,16 @@
       <c r="B34" s="3">
         <v>6154913</v>
       </c>
-      <c r="D34" s="8">
-        <f xml:space="preserve"> B34 / $D$1</f>
+      <c r="D34" s="7">
+        <f t="shared" ref="D34:D52" si="3" xml:space="preserve"> B34 / $D$1</f>
         <v>1.8608412693565752</v>
       </c>
       <c r="E34">
-        <f>IF(D34 &lt; 1, 1, ROUND(D34,0))</f>
+        <f t="shared" ref="E34:E65" si="4">IF(D34 &lt; 1, 1, ROUND(D34,0))</f>
         <v>2</v>
       </c>
-      <c r="F34" s="13">
-        <f>B34 / E34</f>
+      <c r="F34" s="12">
+        <f t="shared" ref="F34:F65" si="5">B34 / E34</f>
         <v>3077456.5</v>
       </c>
     </row>
@@ -1333,16 +1333,16 @@
       <c r="B35" s="3">
         <v>6177224</v>
       </c>
-      <c r="D35" s="8">
-        <f xml:space="preserve"> B35 / $D$1</f>
+      <c r="D35" s="7">
+        <f t="shared" si="3"/>
         <v>1.8675866497641642</v>
       </c>
       <c r="E35">
-        <f>IF(D35 &lt; 1, 1, ROUND(D35,0))</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="F35" s="13">
-        <f>B35 / E35</f>
+      <c r="F35" s="12">
+        <f t="shared" si="5"/>
         <v>3088612</v>
       </c>
       <c r="K35" t="s">
@@ -1356,16 +1356,16 @@
       <c r="B36" s="3">
         <v>6785528</v>
       </c>
-      <c r="D36" s="8">
-        <f xml:space="preserve"> B36 / $D$1</f>
+      <c r="D36" s="7">
+        <f t="shared" si="3"/>
         <v>2.0514978094368814</v>
       </c>
       <c r="E36">
-        <f>IF(D36 &lt; 1, 1, ROUND(D36,0))</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="F36" s="13">
-        <f>B36 / E36</f>
+      <c r="F36" s="12">
+        <f t="shared" si="5"/>
         <v>3392764</v>
       </c>
     </row>
@@ -1376,16 +1376,16 @@
       <c r="B37" s="3">
         <v>6910840</v>
       </c>
-      <c r="D37" s="8">
-        <f xml:space="preserve"> B37 / $D$1</f>
+      <c r="D37" s="7">
+        <f t="shared" si="3"/>
         <v>2.089383924341448</v>
       </c>
       <c r="E37">
-        <f>IF(D37 &lt; 1, 1, ROUND(D37,0))</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="F37" s="13">
-        <f>B37 / E37</f>
+      <c r="F37" s="12">
+        <f t="shared" si="5"/>
         <v>3455420</v>
       </c>
     </row>
@@ -1396,16 +1396,16 @@
       <c r="B38" s="3">
         <v>7029917</v>
       </c>
-      <c r="D38" s="8">
-        <f xml:space="preserve"> B38 / $D$1</f>
+      <c r="D38" s="7">
+        <f t="shared" si="3"/>
         <v>2.1253849849301472</v>
       </c>
       <c r="E38">
-        <f>IF(D38 &lt; 1, 1, ROUND(D38,0))</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="F38" s="13">
-        <f>B38 / E38</f>
+      <c r="F38" s="12">
+        <f t="shared" si="5"/>
         <v>3514958.5</v>
       </c>
     </row>
@@ -1416,16 +1416,16 @@
       <c r="B39" s="3">
         <v>7151502</v>
       </c>
-      <c r="D39" s="8">
-        <f xml:space="preserve"> B39 / $D$1</f>
+      <c r="D39" s="7">
+        <f t="shared" si="3"/>
         <v>2.1621442999252931</v>
       </c>
       <c r="E39">
-        <f>IF(D39 &lt; 1, 1, ROUND(D39,0))</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="F39" s="13">
-        <f>B39 / E39</f>
+      <c r="F39" s="12">
+        <f t="shared" si="5"/>
         <v>3575751</v>
       </c>
     </row>
@@ -1436,16 +1436,16 @@
       <c r="B40" s="3">
         <v>7705281</v>
       </c>
-      <c r="D40" s="8">
-        <f xml:space="preserve"> B40 / $D$1</f>
+      <c r="D40" s="7">
+        <f t="shared" si="3"/>
         <v>2.329570682280822</v>
       </c>
       <c r="E40">
-        <f>IF(D40 &lt; 1, 1, ROUND(D40,0))</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="F40" s="13">
-        <f>B40 / E40</f>
+      <c r="F40" s="12">
+        <f t="shared" si="5"/>
         <v>3852640.5</v>
       </c>
     </row>
@@ -1456,16 +1456,16 @@
       <c r="B41" s="3">
         <v>8631393</v>
       </c>
-      <c r="D41" s="8">
-        <f xml:space="preserve"> B41 / $D$1</f>
+      <c r="D41" s="7">
+        <f t="shared" si="3"/>
         <v>2.6095660988929423</v>
       </c>
       <c r="E41">
-        <f>IF(D41 &lt; 1, 1, ROUND(D41,0))</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="F41" s="13">
-        <f>B41 / E41</f>
+      <c r="F41" s="12">
+        <f t="shared" si="5"/>
         <v>2877131</v>
       </c>
     </row>
@@ -1476,16 +1476,16 @@
       <c r="B42" s="3">
         <v>9288994</v>
       </c>
-      <c r="D42" s="8">
-        <f xml:space="preserve"> B42 / $D$1</f>
+      <c r="D42" s="7">
+        <f t="shared" si="3"/>
         <v>2.8083814321998721</v>
       </c>
       <c r="E42">
-        <f>IF(D42 &lt; 1, 1, ROUND(D42,0))</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="F42" s="13">
-        <f>B42 / E42</f>
+      <c r="F42" s="12">
+        <f t="shared" si="5"/>
         <v>3096331.3333333335</v>
       </c>
     </row>
@@ -1496,16 +1496,16 @@
       <c r="B43" s="3">
         <v>10077331</v>
       </c>
-      <c r="D43" s="8">
-        <f xml:space="preserve"> B43 / $D$1</f>
+      <c r="D43" s="7">
+        <f t="shared" si="3"/>
         <v>3.0467227416157412</v>
       </c>
       <c r="E43">
-        <f>IF(D43 &lt; 1, 1, ROUND(D43,0))</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="F43" s="13">
-        <f>B43 / E43</f>
+      <c r="F43" s="12">
+        <f t="shared" si="5"/>
         <v>3359110.3333333335</v>
       </c>
     </row>
@@ -1516,16 +1516,16 @@
       <c r="B44" s="3">
         <v>10439388</v>
       </c>
-      <c r="D44" s="8">
-        <f xml:space="preserve"> B44 / $D$1</f>
+      <c r="D44" s="7">
+        <f t="shared" si="3"/>
         <v>3.1561849886790925</v>
       </c>
       <c r="E44">
-        <f>IF(D44 &lt; 1, 1, ROUND(D44,0))</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="F44" s="13">
-        <f>B44 / E44</f>
+      <c r="F44" s="12">
+        <f t="shared" si="5"/>
         <v>3479796</v>
       </c>
     </row>
@@ -1536,16 +1536,16 @@
       <c r="B45" s="3">
         <v>10711908</v>
       </c>
-      <c r="D45" s="8">
-        <f xml:space="preserve"> B45 / $D$1</f>
+      <c r="D45" s="7">
+        <f t="shared" si="3"/>
         <v>3.2385771301642854</v>
       </c>
       <c r="E45">
-        <f>IF(D45 &lt; 1, 1, ROUND(D45,0))</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="F45" s="13">
-        <f>B45 / E45</f>
+      <c r="F45" s="12">
+        <f t="shared" si="5"/>
         <v>3570636</v>
       </c>
     </row>
@@ -1556,16 +1556,16 @@
       <c r="B46" s="3">
         <v>11799448</v>
       </c>
-      <c r="D46" s="8">
-        <f xml:space="preserve"> B46 / $D$1</f>
+      <c r="D46" s="7">
+        <f t="shared" si="3"/>
         <v>3.5673777670012399</v>
       </c>
       <c r="E46">
-        <f>IF(D46 &lt; 1, 1, ROUND(D46,0))</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="F46" s="13">
-        <f>B46 / E46</f>
+      <c r="F46" s="12">
+        <f t="shared" si="5"/>
         <v>2949862</v>
       </c>
     </row>
@@ -1576,16 +1576,16 @@
       <c r="B47" s="3">
         <v>12812508</v>
       </c>
-      <c r="D47" s="8">
-        <f xml:space="preserve"> B47 / $D$1</f>
+      <c r="D47" s="7">
+        <f t="shared" si="3"/>
         <v>3.8736605457073519</v>
       </c>
       <c r="E47">
-        <f>IF(D47 &lt; 1, 1, ROUND(D47,0))</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="F47" s="13">
-        <f>B47 / E47</f>
+      <c r="F47" s="12">
+        <f t="shared" si="5"/>
         <v>3203127</v>
       </c>
     </row>
@@ -1596,16 +1596,16 @@
       <c r="B48" s="3">
         <v>13002700</v>
       </c>
-      <c r="D48" s="8">
-        <f xml:space="preserve"> B48 / $D$1</f>
+      <c r="D48" s="7">
+        <f t="shared" si="3"/>
         <v>3.9311621095314817</v>
       </c>
       <c r="E48">
-        <f>IF(D48 &lt; 1, 1, ROUND(D48,0))</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="F48" s="13">
-        <f>B48 / E48</f>
+      <c r="F48" s="12">
+        <f t="shared" si="5"/>
         <v>3250675</v>
       </c>
     </row>
@@ -1616,16 +1616,16 @@
       <c r="B49" s="3">
         <v>20201249</v>
       </c>
-      <c r="D49" s="8">
-        <f xml:space="preserve"> B49 / $D$1</f>
+      <c r="D49" s="7">
+        <f t="shared" si="3"/>
         <v>6.1075303309320939</v>
       </c>
       <c r="E49">
-        <f>IF(D49 &lt; 1, 1, ROUND(D49,0))</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="F49" s="13">
-        <f>B49 / E49</f>
+      <c r="F49" s="12">
+        <f t="shared" si="5"/>
         <v>3366874.8333333335</v>
       </c>
     </row>
@@ -1636,16 +1636,16 @@
       <c r="B50" s="3">
         <v>21538187</v>
       </c>
-      <c r="D50" s="8">
-        <f xml:space="preserve"> B50 / $D$1</f>
+      <c r="D50" s="7">
+        <f t="shared" si="3"/>
         <v>6.5117325357351579</v>
       </c>
       <c r="E50">
-        <f>IF(D50 &lt; 1, 1, ROUND(D50,0))</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="F50" s="13">
-        <f>B50 / E50</f>
+      <c r="F50" s="12">
+        <f t="shared" si="5"/>
         <v>3076883.8571428573</v>
       </c>
     </row>
@@ -1656,16 +1656,16 @@
       <c r="B51" s="3">
         <v>29145505</v>
       </c>
-      <c r="D51" s="8">
-        <f xml:space="preserve"> B51 / $D$1</f>
+      <c r="D51" s="7">
+        <f t="shared" si="3"/>
         <v>8.8116856436863387</v>
       </c>
       <c r="E51">
-        <f>IF(D51 &lt; 1, 1, ROUND(D51,0))</f>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="F51" s="13">
-        <f>B51 / E51</f>
+      <c r="F51" s="12">
+        <f t="shared" si="5"/>
         <v>3238389.4444444445</v>
       </c>
     </row>
@@ -1676,16 +1676,16 @@
       <c r="B52" s="3">
         <v>39538223</v>
       </c>
-      <c r="D52" s="8">
-        <f xml:space="preserve"> B52 / $D$1</f>
+      <c r="D52" s="7">
+        <f t="shared" si="3"/>
         <v>11.953760690918513</v>
       </c>
       <c r="E52">
-        <f>IF(D52 &lt; 1, 1, ROUND(D52,0))</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="F52" s="13">
-        <f>B52 / E52</f>
+      <c r="F52" s="12">
+        <f t="shared" si="5"/>
         <v>3294851.9166666665</v>
       </c>
     </row>
@@ -1714,8 +1714,8 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="6"/>
-      <c r="B56" s="6"/>
+      <c r="A56" s="14"/>
+      <c r="B56" s="14"/>
     </row>
     <row r="57" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>

</xml_diff>